<commit_message>
Poprawione wielkości tablic w warstwach.
</commit_message>
<xml_diff>
--- a/02/sprawozdanie/dane/b/Book1.xlsx
+++ b/02/sprawozdanie/dane/b/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
@@ -124,9 +124,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>zbiór treningowy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -399,9 +396,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>zbiór walidacyjny</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln>
               <a:noFill/>
@@ -679,11 +673,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="556417024"/>
-        <c:axId val="556421056"/>
+        <c:axId val="553993344"/>
+        <c:axId val="553993920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="556417024"/>
+        <c:axId val="553993344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -714,12 +708,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="556421056"/>
+        <c:crossAx val="553993920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="556421056"/>
+        <c:axId val="553993920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +745,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="556417024"/>
+        <c:crossAx val="553993344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -815,9 +809,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>zbiór treningowy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -1090,9 +1081,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>zbiór walidacyjny</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln>
               <a:noFill/>
@@ -1370,11 +1358,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74930944"/>
-        <c:axId val="74723840"/>
+        <c:axId val="553996224"/>
+        <c:axId val="553996800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74930944"/>
+        <c:axId val="553996224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1405,12 +1393,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74723840"/>
+        <c:crossAx val="553996800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74723840"/>
+        <c:axId val="553996800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1442,7 +1430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74930944"/>
+        <c:crossAx val="553996224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1506,9 +1494,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>zbiór treningowy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -1781,9 +1766,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>zbiór walidacyjny</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln>
               <a:noFill/>
@@ -2061,11 +2043,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="47900928"/>
-        <c:axId val="47904960"/>
+        <c:axId val="553999104"/>
+        <c:axId val="553999680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47900928"/>
+        <c:axId val="553999104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2096,12 +2078,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47904960"/>
+        <c:crossAx val="553999680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47904960"/>
+        <c:axId val="553999680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,7 +2115,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47900928"/>
+        <c:crossAx val="553999104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2197,9 +2179,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>zbiór treningowy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -2472,9 +2451,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>zbiór walidacyjny</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln>
               <a:noFill/>
@@ -2752,11 +2728,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="556423360"/>
-        <c:axId val="557143680"/>
+        <c:axId val="554763968"/>
+        <c:axId val="554764544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="556423360"/>
+        <c:axId val="554763968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2787,12 +2763,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="557143680"/>
+        <c:crossAx val="554764544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="557143680"/>
+        <c:axId val="554764544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2824,7 +2800,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="556423360"/>
+        <c:crossAx val="554763968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2888,9 +2864,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>zbiór treningowy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -3036,124 +3009,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.204268168084631</c:v>
+                  <c:v>0.22821911607227399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8398917242088602E-2</c:v>
+                  <c:v>0.13580770082973401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0570906014976804E-2</c:v>
+                  <c:v>0.12944822926581301</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.5450693239853506E-2</c:v>
+                  <c:v>0.11094832287359099</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6902487758656E-2</c:v>
+                  <c:v>9.2250235501406305E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.4846549700710899E-2</c:v>
+                  <c:v>7.56888376725635E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.4035430455506405E-2</c:v>
+                  <c:v>7.3799475296737499E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.3460261990466203E-2</c:v>
+                  <c:v>7.2643352280026399E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.3250044012168803E-2</c:v>
+                  <c:v>7.1728497866598795E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.4119723248040998E-2</c:v>
+                  <c:v>7.0605575445656002E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.2230311553164306E-2</c:v>
+                  <c:v>7.0112174351225395E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.2386814725507296E-2</c:v>
+                  <c:v>6.9622543275471599E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.1094399500478198E-2</c:v>
+                  <c:v>6.9388334617776701E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.2316458913577695E-2</c:v>
+                  <c:v>6.7306881432754206E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.2424800339588405E-2</c:v>
+                  <c:v>6.7974744994446903E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.2237571979697097E-2</c:v>
+                  <c:v>6.8190505407139196E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.3037967308458499E-2</c:v>
+                  <c:v>6.7094416431362505E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.0315622962006103E-2</c:v>
+                  <c:v>6.8054299789963094E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.2353848233221699E-2</c:v>
+                  <c:v>6.7846863091447801E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.9628098698217598E-2</c:v>
+                  <c:v>6.7533332979366298E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.10926535115208399</c:v>
+                  <c:v>6.7756185335516597E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.109883327154842</c:v>
+                  <c:v>6.7857339612714201E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.111923906116577</c:v>
+                  <c:v>6.7723888630226894E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.112403097098818</c:v>
+                  <c:v>6.7175353181042896E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.112855355229341</c:v>
+                  <c:v>6.6615042651147205E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.112636840203187</c:v>
+                  <c:v>6.7627098884120995E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.112207362921991</c:v>
+                  <c:v>6.66904258326E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.11203038163111401</c:v>
+                  <c:v>7.20675310280562E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.109966542649665</c:v>
+                  <c:v>7.1659716945553495E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.10964140822155399</c:v>
+                  <c:v>7.5576235793360994E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.109433522823025</c:v>
+                  <c:v>7.5236276742591895E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.10921466481103299</c:v>
+                  <c:v>7.5713243804519395E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.104210518737285</c:v>
+                  <c:v>7.5742945785873803E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.106392217480145</c:v>
+                  <c:v>7.4944605352852106E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.103776609488029</c:v>
+                  <c:v>8.31043416838569E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.101481995001252</c:v>
+                  <c:v>8.3470719972756596E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.108291488250393</c:v>
+                  <c:v>8.2289507768651293E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.101202511554754</c:v>
+                  <c:v>8.7480910251326302E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.103676600063298</c:v>
+                  <c:v>9.1166981958936494E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.8666755273026194E-2</c:v>
+                  <c:v>8.98026978979901E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3163,9 +3136,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>zbiór walidacyjny</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln>
               <a:noFill/>
@@ -3311,124 +3281,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.17384338214652101</c:v>
+                  <c:v>0.22458928136366901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.5337337559677604E-2</c:v>
+                  <c:v>0.16149330886008501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.6622985194712093E-2</c:v>
+                  <c:v>0.161130534752396</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.5671468695665803E-2</c:v>
+                  <c:v>0.14736443915547101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.4429389555196493E-2</c:v>
+                  <c:v>0.11965813797991599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.0876423058894795E-2</c:v>
+                  <c:v>7.8205579819075693E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0041610115372003E-2</c:v>
+                  <c:v>7.2743547711966797E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.1654604258848296E-2</c:v>
+                  <c:v>7.3256712305289698E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.3007520959407999E-2</c:v>
+                  <c:v>7.2956786397808199E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.0890546750463796E-2</c:v>
+                  <c:v>7.1010765120954902E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.3387961301878394E-2</c:v>
+                  <c:v>7.0232752872374599E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.4535717676728003E-2</c:v>
+                  <c:v>6.9834347290627902E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.2429324042045393E-2</c:v>
+                  <c:v>6.8497088288718699E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.9973500673042999E-2</c:v>
+                  <c:v>7.4252671510473794E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.0833176451558394E-2</c:v>
+                  <c:v>6.4461315653746298E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.5524290551631396E-2</c:v>
+                  <c:v>6.50836315260679E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.0873782899296795E-2</c:v>
+                  <c:v>6.3378659696771505E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.14222635844329E-2</c:v>
+                  <c:v>6.4864028286919506E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.3825203539429701E-2</c:v>
+                  <c:v>6.8502991653211706E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.12742717012336899</c:v>
+                  <c:v>6.4087757349053906E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.12086641472175801</c:v>
+                  <c:v>6.5991067256536695E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.121225090932901</c:v>
+                  <c:v>6.4652800343934794E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.11928447239142601</c:v>
+                  <c:v>6.5253340119807796E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.11939776157429299</c:v>
+                  <c:v>6.8848739225259803E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.11770678244408</c:v>
+                  <c:v>7.0780946328651895E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.118649004952085</c:v>
+                  <c:v>6.3828133140722804E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.11772675666408799</c:v>
+                  <c:v>6.1419421442993102E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.119044460239715</c:v>
+                  <c:v>6.7974605800546997E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.11885059647268</c:v>
+                  <c:v>6.3024425569112599E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.118201392237565</c:v>
+                  <c:v>6.9292665841798398E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.118420939426693</c:v>
+                  <c:v>7.0357630448664096E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.119519327032203</c:v>
+                  <c:v>6.6255874650755997E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.119057183437072</c:v>
+                  <c:v>6.3162983644327195E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.11828230818657599</c:v>
+                  <c:v>6.9415962391780203E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.118238399302124</c:v>
+                  <c:v>6.9600247880148097E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.119153171933959</c:v>
+                  <c:v>6.3515201130887405E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.117582079483082</c:v>
+                  <c:v>6.2026542034679097E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.118953231165791</c:v>
+                  <c:v>6.6251542803540397E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.118318444295093</c:v>
+                  <c:v>6.6200241628065898E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.120898021416578</c:v>
+                  <c:v>6.3027689580907695E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3443,11 +3413,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="556420480"/>
-        <c:axId val="557721280"/>
+        <c:axId val="554766848"/>
+        <c:axId val="554767424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="556420480"/>
+        <c:axId val="554766848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3478,12 +3448,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="557721280"/>
+        <c:crossAx val="554767424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="557721280"/>
+        <c:axId val="554767424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3515,7 +3485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="556420480"/>
+        <c:crossAx val="554766848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3579,9 +3549,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>zbiór treningowy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -3854,9 +3821,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>zbiór walidacyjny</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln>
               <a:noFill/>
@@ -4134,11 +4098,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="697060736"/>
-        <c:axId val="697061312"/>
+        <c:axId val="554769728"/>
+        <c:axId val="554983424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="697060736"/>
+        <c:axId val="554769728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4169,12 +4133,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="697061312"/>
+        <c:crossAx val="554983424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="697061312"/>
+        <c:axId val="554983424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4206,7 +4170,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="697060736"/>
+        <c:crossAx val="554769728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4270,9 +4234,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>zbiór treningowy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -4545,9 +4506,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>zbiór walidacyjny</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln>
               <a:noFill/>
@@ -4825,11 +4783,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="696072384"/>
-        <c:axId val="696071808"/>
+        <c:axId val="554985728"/>
+        <c:axId val="554986304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="696072384"/>
+        <c:axId val="554985728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4860,12 +4818,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="696071808"/>
+        <c:crossAx val="554986304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="696071808"/>
+        <c:axId val="554986304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4897,7 +4855,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="696072384"/>
+        <c:crossAx val="554985728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4961,9 +4919,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>zbiór treningowy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -5236,9 +5191,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>zbiór walidacyjny</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln>
               <a:noFill/>
@@ -5516,11 +5468,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="697063616"/>
-        <c:axId val="697063040"/>
+        <c:axId val="554988608"/>
+        <c:axId val="554989184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="697063616"/>
+        <c:axId val="554988608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5551,12 +5503,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="697063040"/>
+        <c:crossAx val="554989184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="697063040"/>
+        <c:axId val="554989184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5588,7 +5540,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="697063616"/>
+        <c:crossAx val="554988608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5652,9 +5604,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>zbiór treningowy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="47625">
               <a:noFill/>
@@ -5927,9 +5876,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>zbiór walidacyjny</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln>
               <a:noFill/>
@@ -6207,11 +6153,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="697062464"/>
-        <c:axId val="697155584"/>
+        <c:axId val="555565056"/>
+        <c:axId val="555565632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="697062464"/>
+        <c:axId val="555565056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6242,12 +6188,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="697155584"/>
+        <c:crossAx val="555565632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="697155584"/>
+        <c:axId val="555565632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6279,7 +6225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="697062464"/>
+        <c:crossAx val="555565056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7031,7 +6977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
@@ -8928,13 +8874,15 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5" customWidth="1"/>
+    <col min="20" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -8953,10 +8901,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.204268168084631</v>
+        <v>0.22821911607227399</v>
       </c>
       <c r="C2">
-        <v>0.17384338214652101</v>
+        <v>0.22458928136366901</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -8964,10 +8912,10 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>9.8398917242088602E-2</v>
+        <v>0.13580770082973401</v>
       </c>
       <c r="C3">
-        <v>9.5337337559677604E-2</v>
+        <v>0.16149330886008501</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -8975,10 +8923,10 @@
         <v>200</v>
       </c>
       <c r="B4">
-        <v>9.0570906014976804E-2</v>
+        <v>0.12944822926581301</v>
       </c>
       <c r="C4">
-        <v>8.6622985194712093E-2</v>
+        <v>0.161130534752396</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -8986,10 +8934,10 @@
         <v>300</v>
       </c>
       <c r="B5">
-        <v>8.5450693239853506E-2</v>
+        <v>0.11094832287359099</v>
       </c>
       <c r="C5">
-        <v>8.5671468695665803E-2</v>
+        <v>0.14736443915547101</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -8997,10 +8945,10 @@
         <v>400</v>
       </c>
       <c r="B6">
-        <v>8.6902487758656E-2</v>
+        <v>9.2250235501406305E-2</v>
       </c>
       <c r="C6">
-        <v>8.4429389555196493E-2</v>
+        <v>0.11965813797991599</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -9008,10 +8956,10 @@
         <v>500</v>
       </c>
       <c r="B7">
-        <v>8.4846549700710899E-2</v>
+        <v>7.56888376725635E-2</v>
       </c>
       <c r="C7">
-        <v>8.0876423058894795E-2</v>
+        <v>7.8205579819075693E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -9019,10 +8967,10 @@
         <v>600</v>
       </c>
       <c r="B8">
-        <v>8.4035430455506405E-2</v>
+        <v>7.3799475296737499E-2</v>
       </c>
       <c r="C8">
-        <v>8.0041610115372003E-2</v>
+        <v>7.2743547711966797E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -9030,10 +8978,10 @@
         <v>700</v>
       </c>
       <c r="B9">
-        <v>8.3460261990466203E-2</v>
+        <v>7.2643352280026399E-2</v>
       </c>
       <c r="C9">
-        <v>8.1654604258848296E-2</v>
+        <v>7.3256712305289698E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -9041,10 +8989,10 @@
         <v>800</v>
       </c>
       <c r="B10">
-        <v>8.3250044012168803E-2</v>
+        <v>7.1728497866598795E-2</v>
       </c>
       <c r="C10">
-        <v>8.3007520959407999E-2</v>
+        <v>7.2956786397808199E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -9052,10 +9000,10 @@
         <v>900</v>
       </c>
       <c r="B11">
-        <v>8.4119723248040998E-2</v>
+        <v>7.0605575445656002E-2</v>
       </c>
       <c r="C11">
-        <v>8.0890546750463796E-2</v>
+        <v>7.1010765120954902E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -9063,10 +9011,10 @@
         <v>1000</v>
       </c>
       <c r="B12">
-        <v>8.2230311553164306E-2</v>
+        <v>7.0112174351225395E-2</v>
       </c>
       <c r="C12">
-        <v>8.3387961301878394E-2</v>
+        <v>7.0232752872374599E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -9074,10 +9022,10 @@
         <v>1100</v>
       </c>
       <c r="B13">
-        <v>8.2386814725507296E-2</v>
+        <v>6.9622543275471599E-2</v>
       </c>
       <c r="C13">
-        <v>8.4535717676728003E-2</v>
+        <v>6.9834347290627902E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -9085,10 +9033,10 @@
         <v>1200</v>
       </c>
       <c r="B14">
-        <v>8.1094399500478198E-2</v>
+        <v>6.9388334617776701E-2</v>
       </c>
       <c r="C14">
-        <v>8.2429324042045393E-2</v>
+        <v>6.8497088288718699E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -9096,10 +9044,10 @@
         <v>1300</v>
       </c>
       <c r="B15">
-        <v>8.2316458913577695E-2</v>
+        <v>6.7306881432754206E-2</v>
       </c>
       <c r="C15">
-        <v>7.9973500673042999E-2</v>
+        <v>7.4252671510473794E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -9107,10 +9055,10 @@
         <v>1400</v>
       </c>
       <c r="B16">
-        <v>8.2424800339588405E-2</v>
+        <v>6.7974744994446903E-2</v>
       </c>
       <c r="C16">
-        <v>8.0833176451558394E-2</v>
+        <v>6.4461315653746298E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -9118,10 +9066,10 @@
         <v>1500</v>
       </c>
       <c r="B17">
-        <v>8.2237571979697097E-2</v>
+        <v>6.8190505407139196E-2</v>
       </c>
       <c r="C17">
-        <v>8.5524290551631396E-2</v>
+        <v>6.50836315260679E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -9129,10 +9077,10 @@
         <v>1600</v>
       </c>
       <c r="B18">
-        <v>8.3037967308458499E-2</v>
+        <v>6.7094416431362505E-2</v>
       </c>
       <c r="C18">
-        <v>8.0873782899296795E-2</v>
+        <v>6.3378659696771505E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -9140,10 +9088,10 @@
         <v>1700</v>
       </c>
       <c r="B19">
-        <v>8.0315622962006103E-2</v>
+        <v>6.8054299789963094E-2</v>
       </c>
       <c r="C19">
-        <v>8.14222635844329E-2</v>
+        <v>6.4864028286919506E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -9151,10 +9099,10 @@
         <v>1800</v>
       </c>
       <c r="B20">
-        <v>8.2353848233221699E-2</v>
+        <v>6.7846863091447801E-2</v>
       </c>
       <c r="C20">
-        <v>7.3825203539429701E-2</v>
+        <v>6.8502991653211706E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -9162,10 +9110,10 @@
         <v>1900</v>
       </c>
       <c r="B21">
-        <v>8.9628098698217598E-2</v>
+        <v>6.7533332979366298E-2</v>
       </c>
       <c r="C21">
-        <v>0.12742717012336899</v>
+        <v>6.4087757349053906E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -9173,10 +9121,10 @@
         <v>2000</v>
       </c>
       <c r="B22">
-        <v>0.10926535115208399</v>
+        <v>6.7756185335516597E-2</v>
       </c>
       <c r="C22">
-        <v>0.12086641472175801</v>
+        <v>6.5991067256536695E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -9184,10 +9132,10 @@
         <v>2100</v>
       </c>
       <c r="B23">
-        <v>0.109883327154842</v>
+        <v>6.7857339612714201E-2</v>
       </c>
       <c r="C23">
-        <v>0.121225090932901</v>
+        <v>6.4652800343934794E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -9195,10 +9143,10 @@
         <v>2200</v>
       </c>
       <c r="B24">
-        <v>0.111923906116577</v>
+        <v>6.7723888630226894E-2</v>
       </c>
       <c r="C24">
-        <v>0.11928447239142601</v>
+        <v>6.5253340119807796E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -9206,10 +9154,10 @@
         <v>2300</v>
       </c>
       <c r="B25">
-        <v>0.112403097098818</v>
+        <v>6.7175353181042896E-2</v>
       </c>
       <c r="C25">
-        <v>0.11939776157429299</v>
+        <v>6.8848739225259803E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -9217,10 +9165,10 @@
         <v>2400</v>
       </c>
       <c r="B26">
-        <v>0.112855355229341</v>
+        <v>6.6615042651147205E-2</v>
       </c>
       <c r="C26">
-        <v>0.11770678244408</v>
+        <v>7.0780946328651895E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -9228,10 +9176,10 @@
         <v>2500</v>
       </c>
       <c r="B27">
-        <v>0.112636840203187</v>
+        <v>6.7627098884120995E-2</v>
       </c>
       <c r="C27">
-        <v>0.118649004952085</v>
+        <v>6.3828133140722804E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -9239,10 +9187,10 @@
         <v>2600</v>
       </c>
       <c r="B28">
-        <v>0.112207362921991</v>
+        <v>6.66904258326E-2</v>
       </c>
       <c r="C28">
-        <v>0.11772675666408799</v>
+        <v>6.1419421442993102E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -9250,10 +9198,10 @@
         <v>2700</v>
       </c>
       <c r="B29">
-        <v>0.11203038163111401</v>
+        <v>7.20675310280562E-2</v>
       </c>
       <c r="C29">
-        <v>0.119044460239715</v>
+        <v>6.7974605800546997E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -9261,10 +9209,10 @@
         <v>2800</v>
       </c>
       <c r="B30">
-        <v>0.109966542649665</v>
+        <v>7.1659716945553495E-2</v>
       </c>
       <c r="C30">
-        <v>0.11885059647268</v>
+        <v>6.3024425569112599E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -9272,10 +9220,10 @@
         <v>2900</v>
       </c>
       <c r="B31">
-        <v>0.10964140822155399</v>
+        <v>7.5576235793360994E-2</v>
       </c>
       <c r="C31">
-        <v>0.118201392237565</v>
+        <v>6.9292665841798398E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -9283,10 +9231,10 @@
         <v>3000</v>
       </c>
       <c r="B32">
-        <v>0.109433522823025</v>
+        <v>7.5236276742591895E-2</v>
       </c>
       <c r="C32">
-        <v>0.118420939426693</v>
+        <v>7.0357630448664096E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -9294,10 +9242,10 @@
         <v>3100</v>
       </c>
       <c r="B33">
-        <v>0.10921466481103299</v>
+        <v>7.5713243804519395E-2</v>
       </c>
       <c r="C33">
-        <v>0.119519327032203</v>
+        <v>6.6255874650755997E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -9305,10 +9253,10 @@
         <v>3200</v>
       </c>
       <c r="B34">
-        <v>0.104210518737285</v>
+        <v>7.5742945785873803E-2</v>
       </c>
       <c r="C34">
-        <v>0.119057183437072</v>
+        <v>6.3162983644327195E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -9316,10 +9264,10 @@
         <v>3300</v>
       </c>
       <c r="B35">
-        <v>0.106392217480145</v>
+        <v>7.4944605352852106E-2</v>
       </c>
       <c r="C35">
-        <v>0.11828230818657599</v>
+        <v>6.9415962391780203E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -9327,10 +9275,10 @@
         <v>3400</v>
       </c>
       <c r="B36">
-        <v>0.103776609488029</v>
+        <v>8.31043416838569E-2</v>
       </c>
       <c r="C36">
-        <v>0.118238399302124</v>
+        <v>6.9600247880148097E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -9338,10 +9286,10 @@
         <v>3500</v>
       </c>
       <c r="B37">
-        <v>0.101481995001252</v>
+        <v>8.3470719972756596E-2</v>
       </c>
       <c r="C37">
-        <v>0.119153171933959</v>
+        <v>6.3515201130887405E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -9349,10 +9297,10 @@
         <v>3600</v>
       </c>
       <c r="B38">
-        <v>0.108291488250393</v>
+        <v>8.2289507768651293E-2</v>
       </c>
       <c r="C38">
-        <v>0.117582079483082</v>
+        <v>6.2026542034679097E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -9360,10 +9308,10 @@
         <v>3700</v>
       </c>
       <c r="B39">
-        <v>0.101202511554754</v>
+        <v>8.7480910251326302E-2</v>
       </c>
       <c r="C39">
-        <v>0.118953231165791</v>
+        <v>6.6251542803540397E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -9371,10 +9319,10 @@
         <v>3800</v>
       </c>
       <c r="B40">
-        <v>0.103676600063298</v>
+        <v>9.1166981958936494E-2</v>
       </c>
       <c r="C40">
-        <v>0.118318444295093</v>
+        <v>6.6200241628065898E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -9382,10 +9330,10 @@
         <v>3900</v>
       </c>
       <c r="B41">
-        <v>9.8666755273026194E-2</v>
+        <v>8.98026978979901E-2</v>
       </c>
       <c r="C41">
-        <v>0.120898021416578</v>
+        <v>6.3027689580907695E-2</v>
       </c>
     </row>
   </sheetData>
@@ -10823,7 +10771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>